<commit_message>
Changing the excel files
</commit_message>
<xml_diff>
--- a/Excel/Groups.xlsx
+++ b/Excel/Groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\Arbeit Bim+\Node js RESTful\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD1DC7-943A-4535-9567-015238E029CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B708C70-C58E-4BE9-AA43-09AC36D0F9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6870" yWindow="2190" windowWidth="17280" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Guest Group</t>
   </si>
@@ -38,13 +38,24 @@
   <si>
     <t>Gruppe_02</t>
   </si>
+  <si>
+    <t>Gruppe_03</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -68,12 +79,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,23 +413,140 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>